<commit_message>
seems to work fine with fixed datapoints
</commit_message>
<xml_diff>
--- a/inputs/Y.xlsx
+++ b/inputs/Y.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gabriele/Desktop/Poli/OMGP_python/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{37D25A38-A2E9-3342-B7A3-A927093185B5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2AC20F53-56E2-E54F-A9AD-EAD8609F661D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{11A499D1-DA57-7D4C-BE66-4CED774D7DD4}"/>
   </bookViews>
@@ -384,8 +384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD032271-4E93-874A-BCBE-ABCEF284B635}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -398,482 +398,482 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2.0467565532605199</v>
+        <v>0.26414840555765901</v>
       </c>
       <c r="B2">
-        <v>-1.40209358158662</v>
+        <v>0.35941461585450202</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>0.18231931822052699</v>
+        <v>0.271378936151633</v>
       </c>
       <c r="B3">
-        <v>-2.4229724074766201</v>
+        <v>0.41116652981444501</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2.0366661119180201</v>
+        <v>-6.5547541000036694E-2</v>
       </c>
       <c r="B4">
-        <v>-1.4697136527802701</v>
+        <v>-0.71887381464772804</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>0.32282308970261198</v>
+        <v>0.346458836375797</v>
       </c>
       <c r="B5">
-        <v>-2.43999924089721</v>
+        <v>0.43144065998307501</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1.98571599610961</v>
+        <v>-0.51127056297027695</v>
       </c>
       <c r="B6">
-        <v>-1.3810812698983399</v>
+        <v>0.86437608247204101</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>0.130629558769462</v>
+        <v>0.31146104398476898</v>
       </c>
       <c r="B7">
-        <v>1.0920171580529801</v>
+        <v>0.46994230031891698</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2.0580918283965399</v>
+        <v>0.37193867060387098</v>
       </c>
       <c r="B8">
-        <v>-1.46481129169536</v>
+        <v>0.36991944597900001</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1.9085201397667999</v>
+        <v>0.31225567565283202</v>
       </c>
       <c r="B9">
-        <v>-1.3922028578739201</v>
+        <v>0.41722736181888798</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1.91107156432283</v>
+        <v>0.388181492458542</v>
       </c>
       <c r="B10">
-        <v>-1.4482116465847099</v>
+        <v>0.52919279187456403</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>0.22293462694959701</v>
+        <v>0.40284164321316501</v>
       </c>
       <c r="B11">
-        <v>1.0275410332600901</v>
+        <v>0.56209011030899703</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>0.31649371343444299</v>
+        <v>0.409401198293665</v>
       </c>
       <c r="B12">
-        <v>1.08359364940307</v>
+        <v>0.51088453949406498</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>0.217694790753894</v>
+        <v>-0.22791335484278799</v>
       </c>
       <c r="B13">
-        <v>-2.4229059487811</v>
+        <v>0.86070396461224696</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>0.18901794032664501</v>
+        <v>0.45872821777710099</v>
       </c>
       <c r="B14">
-        <v>0.99897517197365204</v>
+        <v>0.493670887818288</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1.8875476517443399</v>
+        <v>0.10716266871801999</v>
       </c>
       <c r="B15">
-        <v>-1.48267395723031</v>
+        <v>-0.53640631238274905</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>0.33387433195768801</v>
+        <v>0.11061039706365799</v>
       </c>
       <c r="B16">
-        <v>1.0073589887401999</v>
+        <v>-0.475687308016153</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>0.27471291339333798</v>
+        <v>-5.1356342163461799E-2</v>
       </c>
       <c r="B17">
-        <v>1.0049810729667801</v>
+        <v>0.84676823082946395</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>0.362757434374124</v>
+        <v>-5.1044244813667303E-2</v>
       </c>
       <c r="B18">
-        <v>0.98845028654771905</v>
+        <v>0.87672441076789198</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>0.35315522195393201</v>
+        <v>0.52843820733352898</v>
       </c>
       <c r="B19">
-        <v>1.0158883660947799</v>
+        <v>0.69679051663454905</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>0.36778814064277199</v>
+        <v>0.29546124552831599</v>
       </c>
       <c r="B20">
-        <v>1.07130447841462</v>
+        <v>-0.47462798371213</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>1.8690030997927001</v>
+        <v>2.09461948990525E-2</v>
       </c>
       <c r="B21">
-        <v>-1.40504187387962</v>
+        <v>0.93664169561454502</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1.8108896050516401</v>
+        <v>0.52695084887657195</v>
       </c>
       <c r="B22">
-        <v>-1.3889439331664499</v>
+        <v>0.494141354139011</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1.7869192740176401</v>
+        <v>0.12826412838880299</v>
       </c>
       <c r="B23">
-        <v>-1.4701099610914501</v>
+        <v>0.94446980731872998</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1.79183441688276</v>
+        <v>0.58410647169722396</v>
       </c>
       <c r="B24">
-        <v>-1.40660379738782</v>
+        <v>0.63599637314864199</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>0.48517734135660801</v>
+        <v>0.24744363663455499</v>
       </c>
       <c r="B25">
-        <v>0.85966239223855301</v>
+        <v>-0.36867334299421001</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>1.82538516570329</v>
+        <v>0.31962888565361203</v>
       </c>
       <c r="B26">
-        <v>-1.46031987521493</v>
+        <v>-0.40188636951079798</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>0.50087950879763798</v>
+        <v>0.38544444797438898</v>
       </c>
       <c r="B27">
-        <v>0.87163653489295601</v>
+        <v>-0.43673526980614003</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>1.78307200764609</v>
+        <v>0.191497798049511</v>
       </c>
       <c r="B28">
-        <v>-1.42011584473887</v>
+        <v>0.83587727740086504</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>1.7072979615738899</v>
+        <v>0.376998998884641</v>
       </c>
       <c r="B29">
-        <v>-1.4821113003889701</v>
+        <v>-0.340993601927503</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>0.16462970321911599</v>
+        <v>0.35650515876504502</v>
       </c>
       <c r="B30">
-        <v>-2.2631615637084002</v>
+        <v>-0.397708641622457</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>4.6368831372933399E-2</v>
+        <v>0.64964935649854305</v>
       </c>
       <c r="B31">
-        <v>-2.18707738684079</v>
+        <v>0.63008007858277204</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>0.118422254644482</v>
+        <v>0.179240247036004</v>
       </c>
       <c r="B32">
-        <v>-2.2087584168971501</v>
+        <v>0.94258011789009999</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>4.8430071927797698E-2</v>
+        <v>0.59080694466747397</v>
       </c>
       <c r="B33">
-        <v>-2.2590598953966001</v>
+        <v>0.67920894131419096</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>0.20910065655899701</v>
+        <v>0.44552674513273999</v>
       </c>
       <c r="B34">
-        <v>-2.2669086856597902</v>
+        <v>-0.26788958559526399</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>1.67096985141279</v>
+        <v>0.275687287834262</v>
       </c>
       <c r="B35">
-        <v>-1.4371109876386201</v>
+        <v>0.95676659032179101</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>1.57292973487359</v>
+        <v>0.73248862681243299</v>
       </c>
       <c r="B36">
-        <v>-1.5157999285677499</v>
+        <v>0.66563796441891898</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>1.5266539533535901</v>
+        <v>0.53609468249343495</v>
       </c>
       <c r="B37">
-        <v>-1.47163911847935</v>
+        <v>-0.21193407703377101</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>0.663853492296407</v>
+        <v>0.43605508259398601</v>
       </c>
       <c r="B38">
-        <v>0.61054786238987702</v>
+        <v>-0.114185160947856</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>8.9232840516255907E-2</v>
+        <v>0.54850407962411596</v>
       </c>
       <c r="B39">
-        <v>-2.1372235210260402</v>
+        <v>0.93665946296306701</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>0.52573878007050601</v>
+        <v>0.61532646732354102</v>
       </c>
       <c r="B40">
-        <v>0.61156616214570803</v>
+        <v>-0.15443916789272399</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>-7.3489586633194506E-2</v>
+        <v>0.74791794179379001</v>
       </c>
       <c r="B41">
-        <v>-2.1083103719236398</v>
+        <v>0.718970319128864</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>-1.1638411840309001E-2</v>
+        <v>0.54695790073710604</v>
       </c>
       <c r="B42">
-        <v>-2.1011585973103202</v>
+        <v>-8.7612507926575198E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>0.61778439720232203</v>
+        <v>0.48339134177481002</v>
       </c>
       <c r="B43">
-        <v>0.61956183557956801</v>
+        <v>0.98224145019473397</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>0.60496603928399095</v>
+        <v>0.54189500528274603</v>
       </c>
       <c r="B44">
-        <v>0.474053235754966</v>
+        <v>-4.1993714615152097E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>-2.0647925185417599E-2</v>
+        <v>0.70556632193148305</v>
       </c>
       <c r="B45">
-        <v>-2.0811921899802699</v>
+        <v>0.73576031740603498</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>-3.6439631566006603E-2</v>
+        <v>0.60769370791829402</v>
       </c>
       <c r="B46">
-        <v>-2.03090206329215</v>
+        <v>1.00440627182139</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>0.53433663861250802</v>
+        <v>0.54699846975601096</v>
       </c>
       <c r="B47">
-        <v>0.48843871231004399</v>
+        <v>0.90550591214320797</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>-3.30458000607168E-2</v>
+        <v>0.59461783613719499</v>
       </c>
       <c r="B48">
-        <v>-2.1044401473784502</v>
+        <v>1.0156646003818299</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>-9.3618698886635598E-2</v>
+        <v>0.62287353251576405</v>
       </c>
       <c r="B49">
-        <v>-2.0715487017756899</v>
+        <v>0.96121649185663505</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>0.61094223094271105</v>
+        <v>0.81814569543908</v>
       </c>
       <c r="B50">
-        <v>0.51441189645266705</v>
+        <v>0.84718049266307804</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>0.58772452836255895</v>
+        <v>0.63839168460175699</v>
       </c>
       <c r="B51">
-        <v>0.48839324905056702</v>
+        <v>1.00723038864112</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>-6.5433132236387304E-2</v>
+        <v>0.63700747690897197</v>
       </c>
       <c r="B52">
-        <v>-1.9342130722641</v>
+        <v>1.0023479169173899</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>1.2750216480653001</v>
+        <v>0.52509110614332999</v>
       </c>
       <c r="B53">
-        <v>-1.4524273243750501</v>
+        <v>4.74836140996691E-2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>0.531581506937293</v>
+        <v>0.51216904119440898</v>
       </c>
       <c r="B54">
-        <v>0.36706978267601298</v>
+        <v>0.12768716291749399</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>1.1706029580278099</v>
+        <v>0.59853883751914305</v>
       </c>
       <c r="B55">
-        <v>-1.38576265393398</v>
+        <v>1.02209103726113</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>0.52942627385825702</v>
+        <v>0.53688581686713299</v>
       </c>
       <c r="B56">
-        <v>0.35644667518701001</v>
+        <v>0.136950742577372</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>2.2871020451547999E-2</v>
+        <v>0.59904327139480495</v>
       </c>
       <c r="B57">
-        <v>-1.9135579638922</v>
+        <v>1.0010626649354299</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>-0.17117501767496901</v>
+        <v>0.801738483596803</v>
       </c>
       <c r="B58">
-        <v>-1.97415309199683</v>
+        <v>0.79266155450644704</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>-0.15324084748394201</v>
+        <v>0.44797841800089</v>
       </c>
       <c r="B59">
-        <v>-1.96105837988395</v>
+        <v>0.108373932416459</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>-0.22875098643321601</v>
+        <v>0.60013527650117005</v>
       </c>
       <c r="B60">
-        <v>-1.9079751165671901</v>
+        <v>1.0359568929509</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>1.1848040507447499</v>
+        <v>0.53113098160141003</v>
       </c>
       <c r="B61">
-        <v>-1.3753567913018501</v>
+        <v>0.20359310820405699</v>
       </c>
     </row>
   </sheetData>

</xml_diff>